<commit_message>
Update slides for first 2 units
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_viz_MA/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B40DE2-2D9A-B24D-B3E2-26879C603A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58406ABA-6F91-6340-BD70-80593BBBDE21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -135,9 +135,6 @@
     <t>inflation</t>
   </si>
   <si>
-    <t>mobility</t>
-  </si>
-  <si>
     <t>06_labour.R</t>
   </si>
   <si>
@@ -145,6 +142,18 @@
   </si>
   <si>
     <t>Maps</t>
+  </si>
+  <si>
+    <t>empstatus</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>01_introduction</t>
+  </si>
+  <si>
+    <t>02_visualization</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,6 +581,9 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
@@ -592,6 +604,9 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
@@ -639,7 +654,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -671,16 +686,16 @@
         <v>31</v>
       </c>
       <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
         <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -743,7 +758,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>

</xml_diff>